<commit_message>
Should Change Request urls in control.html, mock_generator.py when test on Server..
</commit_message>
<xml_diff>
--- a/Plant_Status_fixed.xlsx
+++ b/Plant_Status_fixed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desewenkdk\smartfarmDjango-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E294C5C7-A6C4-49BD-8695-BED73010D7CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E8941A-C27C-4F50-8EDF-9889F9972495}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1694,15 +1694,15 @@
     <xf numFmtId="49" fontId="20" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2152,44 +2152,44 @@
     <row r="1" spans="1:34" ht="41.4">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="67" t="s">
         <v>328</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66" t="s">
+      <c r="D1" s="67"/>
+      <c r="E1" s="67" t="s">
         <v>334</v>
       </c>
-      <c r="F1" s="66"/>
+      <c r="F1" s="67"/>
       <c r="G1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="67" t="s">
+      <c r="H1" s="63" t="s">
         <v>327</v>
       </c>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67" t="s">
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63" t="s">
         <v>316</v>
       </c>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67" t="s">
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63" t="s">
         <v>360</v>
       </c>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67" t="s">
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67" t="s">
+      <c r="R1" s="63"/>
+      <c r="S1" s="63" t="s">
         <v>340</v>
       </c>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67" t="s">
+      <c r="T1" s="63"/>
+      <c r="U1" s="63" t="s">
         <v>338</v>
       </c>
-      <c r="V1" s="67"/>
+      <c r="V1" s="63"/>
       <c r="W1" s="4" t="s">
         <v>292</v>
       </c>
@@ -2208,15 +2208,15 @@
     <row r="2" spans="1:34" ht="28.8">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="67" t="s">
         <v>331</v>
       </c>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66" t="s">
+      <c r="D2" s="67"/>
+      <c r="E2" s="67" t="s">
         <v>347</v>
       </c>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
       <c r="H2" s="4" t="s">
         <v>359</v>
       </c>
@@ -2336,7 +2336,7 @@
       <c r="A4" s="12" t="s">
         <v>339</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="64" t="s">
         <v>307</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -2417,7 +2417,7 @@
       <c r="A5" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="B5" s="64"/>
+      <c r="B5" s="65"/>
       <c r="C5" s="3" t="s">
         <v>308</v>
       </c>
@@ -2496,7 +2496,7 @@
       <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="64"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="3" t="s">
         <v>308</v>
       </c>
@@ -2575,7 +2575,7 @@
       <c r="A7" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="B7" s="64"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="3" t="s">
         <v>308</v>
       </c>
@@ -2654,7 +2654,7 @@
       <c r="A8" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="64"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="3" t="s">
         <v>308</v>
       </c>
@@ -2733,7 +2733,7 @@
       <c r="A9" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="B9" s="64"/>
+      <c r="B9" s="65"/>
       <c r="C9" s="3" t="s">
         <v>308</v>
       </c>
@@ -2812,7 +2812,7 @@
       <c r="A10" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="B10" s="64"/>
+      <c r="B10" s="65"/>
       <c r="C10" s="3" t="s">
         <v>308</v>
       </c>
@@ -2891,7 +2891,7 @@
       <c r="A11" s="19" t="s">
         <v>365</v>
       </c>
-      <c r="B11" s="65"/>
+      <c r="B11" s="66"/>
       <c r="C11" s="3" t="s">
         <v>308</v>
       </c>
@@ -2995,7 +2995,7 @@
       <c r="A13" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="64" t="s">
         <v>310</v>
       </c>
       <c r="C13" s="16"/>
@@ -3027,7 +3027,7 @@
       <c r="A14" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="B14" s="64"/>
+      <c r="B14" s="65"/>
       <c r="C14" s="3" t="s">
         <v>314</v>
       </c>
@@ -3106,7 +3106,7 @@
       <c r="A15" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="B15" s="64"/>
+      <c r="B15" s="65"/>
       <c r="C15" s="3" t="s">
         <v>314</v>
       </c>
@@ -3185,7 +3185,7 @@
       <c r="A16" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="64"/>
+      <c r="B16" s="65"/>
       <c r="C16" s="3" t="s">
         <v>317</v>
       </c>
@@ -3264,7 +3264,7 @@
       <c r="A17" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="B17" s="64"/>
+      <c r="B17" s="65"/>
       <c r="C17" s="3" t="s">
         <v>317</v>
       </c>
@@ -3343,7 +3343,7 @@
       <c r="A18" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="64"/>
+      <c r="B18" s="65"/>
       <c r="C18" s="3" t="s">
         <v>313</v>
       </c>
@@ -3422,7 +3422,7 @@
       <c r="A19" s="28" t="s">
         <v>329</v>
       </c>
-      <c r="B19" s="64"/>
+      <c r="B19" s="65"/>
       <c r="C19" s="3" t="s">
         <v>313</v>
       </c>
@@ -3501,7 +3501,7 @@
       <c r="A20" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="B20" s="64"/>
+      <c r="B20" s="65"/>
       <c r="C20" s="3" t="s">
         <v>295</v>
       </c>
@@ -3580,7 +3580,7 @@
       <c r="A21" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="64"/>
+      <c r="B21" s="65"/>
       <c r="C21" s="3" t="s">
         <v>313</v>
       </c>
@@ -3659,7 +3659,7 @@
       <c r="A22" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="65"/>
+      <c r="B22" s="66"/>
       <c r="C22" s="4">
         <v>4</v>
       </c>
@@ -3761,7 +3761,7 @@
       <c r="A24" s="12" t="s">
         <v>367</v>
       </c>
-      <c r="B24" s="63" t="s">
+      <c r="B24" s="64" t="s">
         <v>293</v>
       </c>
       <c r="C24" s="16"/>
@@ -3793,7 +3793,7 @@
       <c r="A25" s="33" t="s">
         <v>336</v>
       </c>
-      <c r="B25" s="64"/>
+      <c r="B25" s="65"/>
       <c r="C25" s="3" t="s">
         <v>308</v>
       </c>
@@ -3872,7 +3872,7 @@
       <c r="A26" s="33" t="s">
         <v>348</v>
       </c>
-      <c r="B26" s="64"/>
+      <c r="B26" s="65"/>
       <c r="C26" s="3" t="s">
         <v>313</v>
       </c>
@@ -3951,7 +3951,7 @@
       <c r="A27" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="64"/>
+      <c r="B27" s="65"/>
       <c r="C27" s="3" t="s">
         <v>295</v>
       </c>
@@ -4030,7 +4030,7 @@
       <c r="A28" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="B28" s="64"/>
+      <c r="B28" s="65"/>
       <c r="C28" s="4">
         <v>7</v>
       </c>
@@ -4109,7 +4109,7 @@
       <c r="A29" s="18" t="s">
         <v>242</v>
       </c>
-      <c r="B29" s="64"/>
+      <c r="B29" s="65"/>
       <c r="C29" s="16"/>
       <c r="D29" s="16"/>
       <c r="E29" s="3"/>
@@ -4139,7 +4139,7 @@
       <c r="A30" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="B30" s="64"/>
+      <c r="B30" s="65"/>
       <c r="C30" s="3" t="s">
         <v>319</v>
       </c>
@@ -4218,7 +4218,7 @@
       <c r="A31" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="64"/>
+      <c r="B31" s="65"/>
       <c r="C31" s="4">
         <v>7</v>
       </c>
@@ -4294,7 +4294,7 @@
       <c r="A32" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="64"/>
+      <c r="B32" s="65"/>
       <c r="C32" s="3" t="s">
         <v>314</v>
       </c>
@@ -4373,7 +4373,7 @@
       <c r="A33" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="B33" s="64"/>
+      <c r="B33" s="65"/>
       <c r="C33" s="3" t="s">
         <v>311</v>
       </c>
@@ -4452,7 +4452,7 @@
       <c r="A34" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="B34" s="64"/>
+      <c r="B34" s="65"/>
       <c r="C34" s="35" t="s">
         <v>314</v>
       </c>
@@ -4531,7 +4531,7 @@
       <c r="A35" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="B35" s="64"/>
+      <c r="B35" s="65"/>
       <c r="C35" s="3" t="s">
         <v>301</v>
       </c>
@@ -4610,7 +4610,7 @@
       <c r="A36" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B36" s="64"/>
+      <c r="B36" s="65"/>
       <c r="C36" s="3" t="s">
         <v>298</v>
       </c>
@@ -4689,7 +4689,7 @@
       <c r="A37" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="B37" s="64"/>
+      <c r="B37" s="65"/>
       <c r="C37" s="4">
         <v>14</v>
       </c>
@@ -4768,7 +4768,7 @@
       <c r="A38" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="B38" s="64"/>
+      <c r="B38" s="65"/>
       <c r="C38" s="4">
         <v>35</v>
       </c>
@@ -4847,7 +4847,7 @@
       <c r="A39" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="B39" s="65"/>
+      <c r="B39" s="66"/>
       <c r="C39" s="4">
         <v>14</v>
       </c>
@@ -4952,7 +4952,7 @@
       <c r="A41" s="39" t="s">
         <v>239</v>
       </c>
-      <c r="B41" s="63" t="s">
+      <c r="B41" s="64" t="s">
         <v>324</v>
       </c>
       <c r="G41" s="23"/>
@@ -4980,7 +4980,7 @@
       <c r="A42" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B42" s="64"/>
+      <c r="B42" s="65"/>
       <c r="C42" s="4">
         <v>3</v>
       </c>
@@ -5057,7 +5057,7 @@
       <c r="A43" s="18" t="s">
         <v>335</v>
       </c>
-      <c r="B43" s="64"/>
+      <c r="B43" s="65"/>
       <c r="C43" s="4">
         <v>10</v>
       </c>
@@ -5134,7 +5134,7 @@
       <c r="A44" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="64"/>
+      <c r="B44" s="65"/>
       <c r="C44" s="4">
         <v>5</v>
       </c>
@@ -5211,7 +5211,7 @@
       <c r="A45" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B45" s="64"/>
+      <c r="B45" s="65"/>
       <c r="C45" s="4">
         <v>7</v>
       </c>
@@ -5288,7 +5288,7 @@
       <c r="A46" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="B46" s="65"/>
+      <c r="B46" s="66"/>
       <c r="C46" s="4">
         <v>7</v>
       </c>
@@ -29163,11 +29163,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="B24:B39"/>
     <mergeCell ref="B41:B46"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="H1:K1"/>
@@ -29177,6 +29172,11 @@
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="B4:B11"/>
     <mergeCell ref="B13:B22"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="B24:B39"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51166665554046631" footer="0.51166665554046631"/>
@@ -31411,8 +31411,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AD993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>